<commit_message>
Action Card flavor text
It should behave the same way as the Exploration Cards' flavor text.
</commit_message>
<xml_diff>
--- a/Template_Data.xlsx
+++ b/Template_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\TI4Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23AAB79C-B2BC-4DC0-A838-D9BFCDD7D653}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04988ED8-74DA-4FCE-96BE-D81ABF701ABE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1224" yWindow="4668" windowWidth="43692" windowHeight="18972" tabRatio="796" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1224" yWindow="4668" windowWidth="43692" windowHeight="18972" tabRatio="796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Actions" sheetId="14" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3485" uniqueCount="1459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3623" uniqueCount="1459">
   <si>
     <t>Count</t>
   </si>
@@ -4431,10 +4431,10 @@
     <t>&lt;b&gt;After you cast votes on the outcome of an agenda:&lt;/b&gt;&lt;br&gt;&lt;br&gt;Cast 5 additional votes for that outcome.  If that outcome is resolved, you gain 1 command token from your reinforcements.</t>
   </si>
   <si>
-    <t>@[HR,1.75]&lt;ac&gt;&lt;i&gt;The council's research grants would allow for further trips into the ruins of their older worlds.&lt;/i&gt;&lt;/ac&gt;</t>
-  </si>
-  <si>
-    <t>@[HR,1.75]&lt;ac&gt;&lt;i&gt;Elder Junn was a wonder to behold. He knew the name of every senator, made small talk effortlessly, and commanded attention when he spoke.  Magmus hated everything about him.&lt;/i&gt;&lt;/ac&gt;</t>
+    <t>The council's research grants would allow for further trips into the ruins of their older worlds.&lt;/i&gt;&lt;/ac&gt;</t>
+  </si>
+  <si>
+    <t>Elder Junn was a wonder to behold. He knew the name of every senator, made small talk effortlessly, and commanded attention when he spoke.  Magmus hated everything about him.&lt;/i&gt;&lt;/ac&gt;</t>
   </si>
 </sst>
 </file>
@@ -4787,7 +4787,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28CFAFC0-291D-454B-8D29-90443E714B4F}">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
     </sheetView>
@@ -15984,7 +15984,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B804C802-B765-4564-AA28-17FA9BD54FDF}">
   <dimension ref="A1:L63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>

</xml_diff>